<commit_message>
Posodobljen Protokol MT-300 MT-300_TFA.xlsx
</commit_message>
<xml_diff>
--- a/Protokol MT-300 MT-300_TFA.xlsx
+++ b/Protokol MT-300 MT-300_TFA.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="180">
   <si>
     <t>Command explained</t>
   </si>
@@ -706,12 +706,6 @@
     <t>init MACH test, runs mains test and return its result</t>
   </si>
   <si>
-    <t>&gt;MA:ID:MT-300-TFA:MACH:RPE_STARTED:(1.):1:CRC:#013#010</t>
-  </si>
-  <si>
-    <t>&gt;MA:ID:MT-300-TFA:MACH:RPE_STOPPED:(1.):1:CRC:#013#010</t>
-  </si>
-  <si>
     <t>&gt;MA:ID:MT-300-TFA:MACH:START_RPE::1:CRC:#013#010</t>
   </si>
   <si>
@@ -722,6 +716,199 @@
   </si>
   <si>
     <t>start RPE 30A MACH measurement, when return command is transmitted everithing is set</t>
+  </si>
+  <si>
+    <t>&gt;AM:ID:MT-300-TFA:MACH:RPE_STARTED::1:CRC:#013#010</t>
+  </si>
+  <si>
+    <t>&gt;AM:ID:MT-300-TFA:MACH:RPE_STOPPED::1:CRC:#013#010</t>
+  </si>
+  <si>
+    <t>&gt;MA:ID:MT-300-TFA:MACH:START_ALL-PE::1:CRC:#013#010</t>
+  </si>
+  <si>
+    <t>&gt;MA:ID:MT-300-TFA:MACH:START_ONE-PE::1:CRC:#013#010</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Transmitt MACH </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>All Phases to PE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> result. When return message is recieved, measurement has finished.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>start</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> All Phases to PE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> MACH measurement</t>
+    </r>
+  </si>
+  <si>
+    <t>&gt;AM:ID:MT-300-TFA:MACH:RISO_ALL-PE|(1)::1:CRC:#013#010</t>
+  </si>
+  <si>
+    <r>
+      <t>start</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Phases to PE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> MACH measurement</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Transmitt MACH Riso </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Phases to PE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> result (up to 4 fault conditions). When return message is recieved, measurement has finished.</t>
+    </r>
+  </si>
+  <si>
+    <t>&gt;AM:ID:MT-300-TFA:MACH:RISO_ONE-PE|(1),(2)::1:CRC:#013#010</t>
+  </si>
+  <si>
+    <t>&gt;AM:ID:MT-300-TFA:CORD:ALL-PE_STARTED::1:CRC:#013#010</t>
+  </si>
+  <si>
+    <t>&gt;AM:ID:MT-300-TFA:CORD:CONT_STARTED::1:CRC:#013#010</t>
+  </si>
+  <si>
+    <t>&gt;AM:ID:MT-300-TFA:MACH:ALL-PE_STARTED::1:CRC:#013#010</t>
+  </si>
+  <si>
+    <t>&gt;AM:ID:MT-300-TFA:CORD:CW_STARTED::1:CRC:#013#010</t>
+  </si>
+  <si>
+    <t>&gt;AM:ID:MT-300-TFA:MACH:URES_STARTED::1:CRC:#013#010</t>
+  </si>
+  <si>
+    <t>&gt;AM:ID:MT-300-TFA:MACH:ONE-PE_STARTED::1:CRC:#013#010</t>
+  </si>
+  <si>
+    <t>&gt;AM:ID:MT-300-TFA:CORD:ONE-PE_STARTED::1:CRC:#013#010</t>
+  </si>
+  <si>
+    <t>&gt;AM:ID:MT-300-TFA:CORD:PH-PH_STARTED::1:CRC:#013#010</t>
+  </si>
+  <si>
+    <t>&gt;MA:ID:MT-300-TFA:MACH:START_URES:(1.):1:CRC:#013#010</t>
+  </si>
+  <si>
+    <t>1. URES Phase voltage to measure</t>
+  </si>
+  <si>
+    <t>URES Phase voltage to measure</t>
+  </si>
+  <si>
+    <t>"L1-PE"</t>
+  </si>
+  <si>
+    <t>"L2-PE"</t>
+  </si>
+  <si>
+    <t>"L3-PE"</t>
+  </si>
+  <si>
+    <t>"L1-N"</t>
+  </si>
+  <si>
+    <t>"L2-N"</t>
+  </si>
+  <si>
+    <t>"L3-N"</t>
+  </si>
+  <si>
+    <t>&gt;MA:ID:MT-300-TFA:MACH:URES_OPEN::1:CRC:#013#010</t>
+  </si>
+  <si>
+    <t>&gt;AM:ID:MT-300-TFA:MACH:URES_OPENED::1:CRC:#013#010</t>
+  </si>
+  <si>
+    <t>start dedicated URES measurement, when started is returned all is set</t>
+  </si>
+  <si>
+    <t>open input contactors at peak input voltage. Return when the contactors are opened.</t>
   </si>
 </sst>
 </file>
@@ -1157,8 +1344,8 @@
   <dimension ref="A1:AO61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D34" sqref="D34"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1168,7 +1355,7 @@
     <col min="3" max="3" width="71.140625" customWidth="1"/>
     <col min="4" max="4" width="54.7109375" customWidth="1"/>
     <col min="5" max="5" width="115" customWidth="1"/>
-    <col min="7" max="7" width="23.140625" customWidth="1"/>
+    <col min="7" max="7" width="28.7109375" customWidth="1"/>
     <col min="8" max="13" width="15.85546875" customWidth="1"/>
     <col min="14" max="29" width="13.42578125" customWidth="1"/>
     <col min="30" max="37" width="14.85546875" customWidth="1"/>
@@ -1276,6 +1463,9 @@
       <c r="B6" t="s">
         <v>3</v>
       </c>
+      <c r="C6" s="1" t="s">
+        <v>162</v>
+      </c>
       <c r="E6" t="s">
         <v>135</v>
       </c>
@@ -1417,6 +1607,9 @@
         <v>51</v>
       </c>
       <c r="B8" s="4"/>
+      <c r="C8" s="1" t="s">
+        <v>160</v>
+      </c>
       <c r="E8" t="s">
         <v>136</v>
       </c>
@@ -1474,6 +1667,9 @@
       <c r="A10" s="2" t="s">
         <v>52</v>
       </c>
+      <c r="C10" s="1" t="s">
+        <v>159</v>
+      </c>
       <c r="E10" t="s">
         <v>137</v>
       </c>
@@ -1521,8 +1717,32 @@
       <c r="A12" s="2" t="s">
         <v>53</v>
       </c>
+      <c r="C12" s="1" t="s">
+        <v>165</v>
+      </c>
       <c r="E12" t="s">
         <v>138</v>
+      </c>
+      <c r="G12" t="s">
+        <v>169</v>
+      </c>
+      <c r="H12" t="s">
+        <v>170</v>
+      </c>
+      <c r="I12" t="s">
+        <v>171</v>
+      </c>
+      <c r="J12" t="s">
+        <v>172</v>
+      </c>
+      <c r="K12" t="s">
+        <v>173</v>
+      </c>
+      <c r="L12" t="s">
+        <v>174</v>
+      </c>
+      <c r="M12" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="13" spans="1:41" x14ac:dyDescent="0.25">
@@ -1540,6 +1760,9 @@
     <row r="14" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>54</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>166</v>
       </c>
       <c r="E14" t="s">
         <v>139</v>
@@ -1741,34 +1964,94 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="E32" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="E33" t="s">
-        <v>149</v>
+        <v>147</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="E34" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C35" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D35" t="s">
+        <v>56</v>
+      </c>
+      <c r="E35" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C36" s="12"/>
+      <c r="A36" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="E36" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C37" s="12"/>
+      <c r="C37" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D37" t="s">
+        <v>69</v>
+      </c>
+      <c r="E37" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C38" s="12"/>
+      <c r="A38" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="B38" t="s">
+        <v>168</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="E38" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="E39" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="56" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C56" s="5" t="s">

</xml_diff>